<commit_message>
Update tables in main.md
</commit_message>
<xml_diff>
--- a/docs/InhoudGWSWpersleidingen_V1_1.xlsx
+++ b/docs/InhoudGWSWpersleidingen_V1_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\projecten_p4uw\RIONED36 (GWSW modellering)\GWSW persleidingen\GitHub\gwsw-persleidingen\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C664A64-3865-4F46-8B96-8628FFAFECF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5B2E0F-0502-43E3-B31A-1EA2580BE892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchie" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="228">
   <si>
     <t>Persleidingsysteem</t>
   </si>
@@ -709,9 +709,6 @@
   </si>
   <si>
     <t>Algemeen</t>
-  </si>
-  <si>
-    <t>nee</t>
   </si>
   <si>
     <t>Voorziet Risicogebied al in de behoefte? Kunnen ook b.v. dijken of spoorlijnen omvatten. Welicht constructieonderdelen ook onderdeel maken van risicogebied (putten zitten er ook al bij)</t>
@@ -1343,8 +1340,8 @@
   </sheetPr>
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2045,7 +2042,7 @@
         <v>44</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -2215,7 +2212,7 @@
     </row>
     <row r="47" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
-        <v>224</v>
+        <v>44</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="3"/>
@@ -2322,7 +2319,7 @@
         <v>44</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>211</v>
@@ -2431,7 +2428,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>201</v>
@@ -2519,7 +2516,7 @@
     </row>
     <row r="61" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>195</v>
@@ -2542,7 +2539,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>150</v>
@@ -2581,7 +2578,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>196</v>
@@ -2708,7 +2705,7 @@
     </row>
     <row r="71" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>207</v>
@@ -2723,7 +2720,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>208</v>
@@ -2738,7 +2735,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>218</v>
@@ -2753,7 +2750,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>216</v>
@@ -2776,7 +2773,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B75" s="22"/>
       <c r="C75" s="8" t="s">

</xml_diff>